<commit_message>
Deploying to gh-pages from  @ f4a392c38d5a77a60a2cb6ba093f617a24d5915a 🚀
</commit_message>
<xml_diff>
--- a/assets/excel/2022_6-2-2.xlsx
+++ b/assets/excel/2022_6-2-2.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="S:\Hannover\Dez15-Uebergreifende-Analysen\Projekte\Integrationsmonitoring\github\MT_Site\assets\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1B069E9A-8315-482B-9DCC-A6E0A73AFB5F}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F2C8686-BB0E-4D2A-8695-BBA6D212F225}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="14010" xr2:uid="{6D20BA34-5F99-4BCC-BC15-D54A156181FF}"/>
   </bookViews>
@@ -29,9 +29,6 @@
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="379" uniqueCount="116">
-  <si>
-    <t>Migration und Teilhabe in Niedersachsen - Integrationsmonitoring 2021</t>
-  </si>
   <si>
     <t>Indikator 6.2.2: Empfängerinnen und Empfänger von Mindestsicherungsleistungen nach Nationalität und Altersgruppen</t>
   </si>
@@ -390,6 +387,9 @@
   </si>
   <si>
     <t>https://www.integrationsmonitoring.niedersachsen.de</t>
+  </si>
+  <si>
+    <t>Migration und Teilhabe in Niedersachsen - Integrationsmonitoring 2022</t>
   </si>
 </sst>
 </file>
@@ -1279,7 +1279,9 @@
   <sheetPr codeName="Tabelle1"/>
   <dimension ref="B1:O384"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="C1" sqref="C1"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1290,7 +1292,7 @@
   <sheetData>
     <row r="1" spans="2:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C1" s="2" t="s">
-        <v>0</v>
+        <v>115</v>
       </c>
       <c r="D1" s="3"/>
       <c r="E1" s="3"/>
@@ -1309,7 +1311,7 @@
     </row>
     <row r="3" spans="2:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C3" s="6" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D3" s="7"/>
       <c r="E3" s="7"/>
@@ -1323,7 +1325,7 @@
     </row>
     <row r="4" spans="2:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C4" s="7" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D4" s="7"/>
       <c r="E4" s="7"/>
@@ -1356,13 +1358,13 @@
     <row r="7" spans="2:15" s="16" customFormat="1" ht="8.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B7" s="13"/>
       <c r="C7" s="35" t="s">
+        <v>2</v>
+      </c>
+      <c r="D7" s="38" t="s">
         <v>3</v>
       </c>
-      <c r="D7" s="38" t="s">
+      <c r="E7" s="41" t="s">
         <v>4</v>
-      </c>
-      <c r="E7" s="41" t="s">
-        <v>5</v>
       </c>
       <c r="F7" s="42"/>
       <c r="G7" s="42"/>
@@ -1377,12 +1379,12 @@
       <c r="C8" s="36"/>
       <c r="D8" s="39"/>
       <c r="E8" s="43" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F8" s="44"/>
       <c r="G8" s="44"/>
       <c r="H8" s="44" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="I8" s="44"/>
       <c r="J8" s="45"/>
@@ -1394,22 +1396,22 @@
       <c r="C9" s="36"/>
       <c r="D9" s="39"/>
       <c r="E9" s="18" t="s">
+        <v>7</v>
+      </c>
+      <c r="F9" s="19" t="s">
         <v>8</v>
       </c>
-      <c r="F9" s="19" t="s">
+      <c r="G9" s="19" t="s">
         <v>9</v>
       </c>
-      <c r="G9" s="19" t="s">
-        <v>10</v>
-      </c>
       <c r="H9" s="18" t="s">
+        <v>7</v>
+      </c>
+      <c r="I9" s="19" t="s">
         <v>8</v>
       </c>
-      <c r="I9" s="19" t="s">
+      <c r="J9" s="20" t="s">
         <v>9</v>
-      </c>
-      <c r="J9" s="20" t="s">
-        <v>10</v>
       </c>
       <c r="K9" s="15"/>
       <c r="O9" s="5"/>
@@ -1419,7 +1421,7 @@
       <c r="C10" s="37"/>
       <c r="D10" s="40"/>
       <c r="E10" s="46" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F10" s="47"/>
       <c r="G10" s="47"/>
@@ -1434,7 +1436,7 @@
         <v>101</v>
       </c>
       <c r="C12" s="22" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D12" s="22">
         <v>2020</v>
@@ -1463,7 +1465,7 @@
         <v>102</v>
       </c>
       <c r="C13" s="22" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D13" s="22">
         <v>2020</v>
@@ -1492,7 +1494,7 @@
         <v>103</v>
       </c>
       <c r="C14" s="22" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D14" s="22">
         <v>2020</v>
@@ -1521,7 +1523,7 @@
         <v>151</v>
       </c>
       <c r="C15" s="22" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D15" s="22">
         <v>2020</v>
@@ -1550,7 +1552,7 @@
         <v>153</v>
       </c>
       <c r="C16" s="22" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D16" s="22">
         <v>2020</v>
@@ -1579,7 +1581,7 @@
         <v>154</v>
       </c>
       <c r="C17" s="22" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D17" s="22">
         <v>2020</v>
@@ -1608,7 +1610,7 @@
         <v>155</v>
       </c>
       <c r="C18" s="22" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D18" s="22">
         <v>2020</v>
@@ -1637,7 +1639,7 @@
         <v>157</v>
       </c>
       <c r="C19" s="22" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D19" s="22">
         <v>2020</v>
@@ -1666,7 +1668,7 @@
         <v>158</v>
       </c>
       <c r="C20" s="22" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D20" s="22">
         <v>2020</v>
@@ -1695,7 +1697,7 @@
         <v>159</v>
       </c>
       <c r="C21" s="22" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D21" s="22">
         <v>2020</v>
@@ -1724,7 +1726,7 @@
         <v>1</v>
       </c>
       <c r="C22" s="24" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D22" s="24">
         <v>2020</v>
@@ -1753,7 +1755,7 @@
         <v>241</v>
       </c>
       <c r="C23" s="22" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D23" s="22">
         <v>2020</v>
@@ -1782,7 +1784,7 @@
         <v>241001</v>
       </c>
       <c r="C24" s="22" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D24" s="22">
         <v>2020</v>
@@ -1811,7 +1813,7 @@
         <v>241999</v>
       </c>
       <c r="C25" s="22" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D25" s="22">
         <v>2020</v>
@@ -1840,7 +1842,7 @@
         <v>251</v>
       </c>
       <c r="C26" s="22" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D26" s="22">
         <v>2020</v>
@@ -1869,7 +1871,7 @@
         <v>252</v>
       </c>
       <c r="C27" s="22" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D27" s="22">
         <v>2020</v>
@@ -1898,7 +1900,7 @@
         <v>254</v>
       </c>
       <c r="C28" s="22" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D28" s="22">
         <v>2020</v>
@@ -1927,7 +1929,7 @@
         <v>255</v>
       </c>
       <c r="C29" s="22" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D29" s="22">
         <v>2020</v>
@@ -1956,7 +1958,7 @@
         <v>256</v>
       </c>
       <c r="C30" s="22" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D30" s="22">
         <v>2020</v>
@@ -1985,7 +1987,7 @@
         <v>257</v>
       </c>
       <c r="C31" s="22" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D31" s="22">
         <v>2020</v>
@@ -2014,7 +2016,7 @@
         <v>2</v>
       </c>
       <c r="C32" s="24" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D32" s="24">
         <v>2020</v>
@@ -2043,7 +2045,7 @@
         <v>351</v>
       </c>
       <c r="C33" s="22" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D33" s="22">
         <v>2020</v>
@@ -2072,7 +2074,7 @@
         <v>352</v>
       </c>
       <c r="C34" s="22" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D34" s="22">
         <v>2020</v>
@@ -2101,7 +2103,7 @@
         <v>353</v>
       </c>
       <c r="C35" s="22" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D35" s="22">
         <v>2020</v>
@@ -2130,7 +2132,7 @@
         <v>354</v>
       </c>
       <c r="C36" s="22" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D36" s="22">
         <v>2020</v>
@@ -2159,7 +2161,7 @@
         <v>355</v>
       </c>
       <c r="C37" s="22" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D37" s="22">
         <v>2020</v>
@@ -2188,7 +2190,7 @@
         <v>356</v>
       </c>
       <c r="C38" s="22" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D38" s="22">
         <v>2020</v>
@@ -2217,7 +2219,7 @@
         <v>357</v>
       </c>
       <c r="C39" s="22" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D39" s="22">
         <v>2020</v>
@@ -2246,7 +2248,7 @@
         <v>358</v>
       </c>
       <c r="C40" s="22" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D40" s="22">
         <v>2020</v>
@@ -2275,7 +2277,7 @@
         <v>359</v>
       </c>
       <c r="C41" s="22" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D41" s="22">
         <v>2020</v>
@@ -2304,7 +2306,7 @@
         <v>360</v>
       </c>
       <c r="C42" s="22" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D42" s="22">
         <v>2020</v>
@@ -2333,7 +2335,7 @@
         <v>361</v>
       </c>
       <c r="C43" s="22" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D43" s="22">
         <v>2020</v>
@@ -2362,7 +2364,7 @@
         <v>3</v>
       </c>
       <c r="C44" s="24" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D44" s="24">
         <v>2020</v>
@@ -2391,7 +2393,7 @@
         <v>401</v>
       </c>
       <c r="C45" s="22" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D45" s="22">
         <v>2020</v>
@@ -2420,7 +2422,7 @@
         <v>402</v>
       </c>
       <c r="C46" s="22" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D46" s="22">
         <v>2020</v>
@@ -2449,7 +2451,7 @@
         <v>403</v>
       </c>
       <c r="C47" s="22" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D47" s="22">
         <v>2020</v>
@@ -2478,7 +2480,7 @@
         <v>404</v>
       </c>
       <c r="C48" s="22" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D48" s="22">
         <v>2020</v>
@@ -2507,7 +2509,7 @@
         <v>405</v>
       </c>
       <c r="C49" s="22" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D49" s="22">
         <v>2020</v>
@@ -2536,7 +2538,7 @@
         <v>451</v>
       </c>
       <c r="C50" s="22" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D50" s="22">
         <v>2020</v>
@@ -2565,7 +2567,7 @@
         <v>452</v>
       </c>
       <c r="C51" s="22" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D51" s="22">
         <v>2020</v>
@@ -2594,7 +2596,7 @@
         <v>453</v>
       </c>
       <c r="C52" s="22" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D52" s="22">
         <v>2020</v>
@@ -2623,7 +2625,7 @@
         <v>454</v>
       </c>
       <c r="C53" s="22" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D53" s="22">
         <v>2020</v>
@@ -2652,7 +2654,7 @@
         <v>455</v>
       </c>
       <c r="C54" s="22" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D54" s="22">
         <v>2020</v>
@@ -2681,7 +2683,7 @@
         <v>456</v>
       </c>
       <c r="C55" s="22" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D55" s="22">
         <v>2020</v>
@@ -2710,7 +2712,7 @@
         <v>457</v>
       </c>
       <c r="C56" s="22" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D56" s="22">
         <v>2020</v>
@@ -2739,7 +2741,7 @@
         <v>458</v>
       </c>
       <c r="C57" s="22" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D57" s="22">
         <v>2020</v>
@@ -2768,7 +2770,7 @@
         <v>459</v>
       </c>
       <c r="C58" s="22" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D58" s="22">
         <v>2020</v>
@@ -2797,7 +2799,7 @@
         <v>460</v>
       </c>
       <c r="C59" s="22" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D59" s="22">
         <v>2020</v>
@@ -2826,7 +2828,7 @@
         <v>461</v>
       </c>
       <c r="C60" s="22" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D60" s="22">
         <v>2020</v>
@@ -2855,7 +2857,7 @@
         <v>462</v>
       </c>
       <c r="C61" s="22" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D61" s="22">
         <v>2020</v>
@@ -2884,7 +2886,7 @@
         <v>4</v>
       </c>
       <c r="C62" s="24" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D62" s="24">
         <v>2020</v>
@@ -2913,7 +2915,7 @@
         <v>0</v>
       </c>
       <c r="C63" s="24" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D63" s="24">
         <v>2020</v>
@@ -2942,7 +2944,7 @@
         <v>101</v>
       </c>
       <c r="C64" s="22" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D64" s="22">
         <v>2019</v>
@@ -2971,7 +2973,7 @@
         <v>102</v>
       </c>
       <c r="C65" s="22" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D65" s="22">
         <v>2019</v>
@@ -3000,7 +3002,7 @@
         <v>103</v>
       </c>
       <c r="C66" s="22" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D66" s="22">
         <v>2019</v>
@@ -3029,7 +3031,7 @@
         <v>151</v>
       </c>
       <c r="C67" s="22" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D67" s="22">
         <v>2019</v>
@@ -3058,7 +3060,7 @@
         <v>153</v>
       </c>
       <c r="C68" s="22" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D68" s="22">
         <v>2019</v>
@@ -3087,7 +3089,7 @@
         <v>154</v>
       </c>
       <c r="C69" s="22" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D69" s="22">
         <v>2019</v>
@@ -3116,7 +3118,7 @@
         <v>155</v>
       </c>
       <c r="C70" s="22" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D70" s="22">
         <v>2019</v>
@@ -3145,7 +3147,7 @@
         <v>157</v>
       </c>
       <c r="C71" s="22" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D71" s="22">
         <v>2019</v>
@@ -3174,7 +3176,7 @@
         <v>158</v>
       </c>
       <c r="C72" s="22" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D72" s="22">
         <v>2019</v>
@@ -3203,7 +3205,7 @@
         <v>159</v>
       </c>
       <c r="C73" s="22" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D73" s="22">
         <v>2019</v>
@@ -3232,7 +3234,7 @@
         <v>1</v>
       </c>
       <c r="C74" s="24" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D74" s="24">
         <v>2019</v>
@@ -3261,7 +3263,7 @@
         <v>241</v>
       </c>
       <c r="C75" s="22" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D75" s="22">
         <v>2019</v>
@@ -3290,7 +3292,7 @@
         <v>241001</v>
       </c>
       <c r="C76" s="22" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D76" s="22">
         <v>2019</v>
@@ -3319,7 +3321,7 @@
         <v>241999</v>
       </c>
       <c r="C77" s="22" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D77" s="22">
         <v>2019</v>
@@ -3348,7 +3350,7 @@
         <v>251</v>
       </c>
       <c r="C78" s="22" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D78" s="22">
         <v>2019</v>
@@ -3377,7 +3379,7 @@
         <v>252</v>
       </c>
       <c r="C79" s="22" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D79" s="22">
         <v>2019</v>
@@ -3406,7 +3408,7 @@
         <v>254</v>
       </c>
       <c r="C80" s="22" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D80" s="22">
         <v>2019</v>
@@ -3435,7 +3437,7 @@
         <v>255</v>
       </c>
       <c r="C81" s="22" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D81" s="22">
         <v>2019</v>
@@ -3464,7 +3466,7 @@
         <v>256</v>
       </c>
       <c r="C82" s="22" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D82" s="22">
         <v>2019</v>
@@ -3493,7 +3495,7 @@
         <v>257</v>
       </c>
       <c r="C83" s="22" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D83" s="22">
         <v>2019</v>
@@ -3522,7 +3524,7 @@
         <v>2</v>
       </c>
       <c r="C84" s="24" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D84" s="24">
         <v>2019</v>
@@ -3551,7 +3553,7 @@
         <v>351</v>
       </c>
       <c r="C85" s="22" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D85" s="22">
         <v>2019</v>
@@ -3580,7 +3582,7 @@
         <v>352</v>
       </c>
       <c r="C86" s="22" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D86" s="22">
         <v>2019</v>
@@ -3609,7 +3611,7 @@
         <v>353</v>
       </c>
       <c r="C87" s="22" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D87" s="22">
         <v>2019</v>
@@ -3638,7 +3640,7 @@
         <v>354</v>
       </c>
       <c r="C88" s="22" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D88" s="22">
         <v>2019</v>
@@ -3667,7 +3669,7 @@
         <v>355</v>
       </c>
       <c r="C89" s="22" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D89" s="22">
         <v>2019</v>
@@ -3696,7 +3698,7 @@
         <v>356</v>
       </c>
       <c r="C90" s="22" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D90" s="22">
         <v>2019</v>
@@ -3725,7 +3727,7 @@
         <v>357</v>
       </c>
       <c r="C91" s="22" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D91" s="22">
         <v>2019</v>
@@ -3754,7 +3756,7 @@
         <v>358</v>
       </c>
       <c r="C92" s="22" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D92" s="22">
         <v>2019</v>
@@ -3783,7 +3785,7 @@
         <v>359</v>
       </c>
       <c r="C93" s="22" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D93" s="22">
         <v>2019</v>
@@ -3812,7 +3814,7 @@
         <v>360</v>
       </c>
       <c r="C94" s="22" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D94" s="22">
         <v>2019</v>
@@ -3841,7 +3843,7 @@
         <v>361</v>
       </c>
       <c r="C95" s="22" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D95" s="22">
         <v>2019</v>
@@ -3870,7 +3872,7 @@
         <v>3</v>
       </c>
       <c r="C96" s="24" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D96" s="24">
         <v>2019</v>
@@ -3899,7 +3901,7 @@
         <v>401</v>
       </c>
       <c r="C97" s="22" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D97" s="22">
         <v>2019</v>
@@ -3928,7 +3930,7 @@
         <v>402</v>
       </c>
       <c r="C98" s="22" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D98" s="22">
         <v>2019</v>
@@ -3957,7 +3959,7 @@
         <v>403</v>
       </c>
       <c r="C99" s="22" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D99" s="22">
         <v>2019</v>
@@ -3986,7 +3988,7 @@
         <v>404</v>
       </c>
       <c r="C100" s="22" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D100" s="22">
         <v>2019</v>
@@ -4015,7 +4017,7 @@
         <v>405</v>
       </c>
       <c r="C101" s="22" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D101" s="22">
         <v>2019</v>
@@ -4044,7 +4046,7 @@
         <v>451</v>
       </c>
       <c r="C102" s="22" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D102" s="22">
         <v>2019</v>
@@ -4073,7 +4075,7 @@
         <v>452</v>
       </c>
       <c r="C103" s="22" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D103" s="22">
         <v>2019</v>
@@ -4102,7 +4104,7 @@
         <v>453</v>
       </c>
       <c r="C104" s="22" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D104" s="22">
         <v>2019</v>
@@ -4131,7 +4133,7 @@
         <v>454</v>
       </c>
       <c r="C105" s="22" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D105" s="22">
         <v>2019</v>
@@ -4160,7 +4162,7 @@
         <v>455</v>
       </c>
       <c r="C106" s="22" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D106" s="22">
         <v>2019</v>
@@ -4189,7 +4191,7 @@
         <v>456</v>
       </c>
       <c r="C107" s="22" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D107" s="22">
         <v>2019</v>
@@ -4218,7 +4220,7 @@
         <v>457</v>
       </c>
       <c r="C108" s="22" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D108" s="22">
         <v>2019</v>
@@ -4247,7 +4249,7 @@
         <v>458</v>
       </c>
       <c r="C109" s="22" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D109" s="22">
         <v>2019</v>
@@ -4276,7 +4278,7 @@
         <v>459</v>
       </c>
       <c r="C110" s="22" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D110" s="22">
         <v>2019</v>
@@ -4305,7 +4307,7 @@
         <v>460</v>
       </c>
       <c r="C111" s="22" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D111" s="22">
         <v>2019</v>
@@ -4334,7 +4336,7 @@
         <v>461</v>
       </c>
       <c r="C112" s="22" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D112" s="22">
         <v>2019</v>
@@ -4363,7 +4365,7 @@
         <v>462</v>
       </c>
       <c r="C113" s="22" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D113" s="22">
         <v>2019</v>
@@ -4392,7 +4394,7 @@
         <v>4</v>
       </c>
       <c r="C114" s="24" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D114" s="24">
         <v>2019</v>
@@ -4421,7 +4423,7 @@
         <v>0</v>
       </c>
       <c r="C115" s="24" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D115" s="24">
         <v>2019</v>
@@ -4450,7 +4452,7 @@
         <v>101</v>
       </c>
       <c r="C116" s="22" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D116" s="22">
         <v>2018</v>
@@ -4479,7 +4481,7 @@
         <v>102</v>
       </c>
       <c r="C117" s="22" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D117" s="22">
         <v>2018</v>
@@ -4508,7 +4510,7 @@
         <v>103</v>
       </c>
       <c r="C118" s="22" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D118" s="22">
         <v>2018</v>
@@ -4537,7 +4539,7 @@
         <v>151</v>
       </c>
       <c r="C119" s="22" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D119" s="22">
         <v>2018</v>
@@ -4566,7 +4568,7 @@
         <v>153</v>
       </c>
       <c r="C120" s="22" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D120" s="22">
         <v>2018</v>
@@ -4595,7 +4597,7 @@
         <v>154</v>
       </c>
       <c r="C121" s="22" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D121" s="22">
         <v>2018</v>
@@ -4624,7 +4626,7 @@
         <v>155</v>
       </c>
       <c r="C122" s="22" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D122" s="22">
         <v>2018</v>
@@ -4653,7 +4655,7 @@
         <v>157</v>
       </c>
       <c r="C123" s="22" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D123" s="22">
         <v>2018</v>
@@ -4682,7 +4684,7 @@
         <v>158</v>
       </c>
       <c r="C124" s="22" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D124" s="22">
         <v>2018</v>
@@ -4711,7 +4713,7 @@
         <v>159</v>
       </c>
       <c r="C125" s="22" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D125" s="22">
         <v>2018</v>
@@ -4740,7 +4742,7 @@
         <v>1</v>
       </c>
       <c r="C126" s="24" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D126" s="24">
         <v>2018</v>
@@ -4769,7 +4771,7 @@
         <v>241</v>
       </c>
       <c r="C127" s="22" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D127" s="22">
         <v>2018</v>
@@ -4798,7 +4800,7 @@
         <v>241001</v>
       </c>
       <c r="C128" s="22" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D128" s="22">
         <v>2018</v>
@@ -4827,7 +4829,7 @@
         <v>241999</v>
       </c>
       <c r="C129" s="22" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D129" s="22">
         <v>2018</v>
@@ -4856,7 +4858,7 @@
         <v>251</v>
       </c>
       <c r="C130" s="22" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D130" s="22">
         <v>2018</v>
@@ -4885,7 +4887,7 @@
         <v>252</v>
       </c>
       <c r="C131" s="22" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D131" s="22">
         <v>2018</v>
@@ -4914,7 +4916,7 @@
         <v>254</v>
       </c>
       <c r="C132" s="22" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D132" s="22">
         <v>2018</v>
@@ -4943,7 +4945,7 @@
         <v>255</v>
       </c>
       <c r="C133" s="22" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D133" s="22">
         <v>2018</v>
@@ -4972,7 +4974,7 @@
         <v>256</v>
       </c>
       <c r="C134" s="22" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D134" s="22">
         <v>2018</v>
@@ -5001,7 +5003,7 @@
         <v>257</v>
       </c>
       <c r="C135" s="22" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D135" s="22">
         <v>2018</v>
@@ -5030,7 +5032,7 @@
         <v>2</v>
       </c>
       <c r="C136" s="24" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D136" s="24">
         <v>2018</v>
@@ -5059,7 +5061,7 @@
         <v>351</v>
       </c>
       <c r="C137" s="22" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D137" s="22">
         <v>2018</v>
@@ -5088,7 +5090,7 @@
         <v>352</v>
       </c>
       <c r="C138" s="22" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D138" s="22">
         <v>2018</v>
@@ -5117,7 +5119,7 @@
         <v>353</v>
       </c>
       <c r="C139" s="22" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D139" s="22">
         <v>2018</v>
@@ -5146,7 +5148,7 @@
         <v>354</v>
       </c>
       <c r="C140" s="22" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D140" s="22">
         <v>2018</v>
@@ -5175,7 +5177,7 @@
         <v>355</v>
       </c>
       <c r="C141" s="22" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D141" s="22">
         <v>2018</v>
@@ -5204,7 +5206,7 @@
         <v>356</v>
       </c>
       <c r="C142" s="22" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D142" s="22">
         <v>2018</v>
@@ -5233,7 +5235,7 @@
         <v>357</v>
       </c>
       <c r="C143" s="22" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D143" s="22">
         <v>2018</v>
@@ -5262,7 +5264,7 @@
         <v>358</v>
       </c>
       <c r="C144" s="22" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D144" s="22">
         <v>2018</v>
@@ -5291,7 +5293,7 @@
         <v>359</v>
       </c>
       <c r="C145" s="22" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D145" s="22">
         <v>2018</v>
@@ -5320,7 +5322,7 @@
         <v>360</v>
       </c>
       <c r="C146" s="22" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D146" s="22">
         <v>2018</v>
@@ -5349,7 +5351,7 @@
         <v>361</v>
       </c>
       <c r="C147" s="22" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D147" s="22">
         <v>2018</v>
@@ -5378,7 +5380,7 @@
         <v>3</v>
       </c>
       <c r="C148" s="24" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D148" s="24">
         <v>2018</v>
@@ -5407,7 +5409,7 @@
         <v>401</v>
       </c>
       <c r="C149" s="22" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D149" s="22">
         <v>2018</v>
@@ -5436,7 +5438,7 @@
         <v>402</v>
       </c>
       <c r="C150" s="22" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D150" s="22">
         <v>2018</v>
@@ -5465,7 +5467,7 @@
         <v>403</v>
       </c>
       <c r="C151" s="22" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D151" s="22">
         <v>2018</v>
@@ -5494,7 +5496,7 @@
         <v>404</v>
       </c>
       <c r="C152" s="22" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D152" s="22">
         <v>2018</v>
@@ -5523,7 +5525,7 @@
         <v>405</v>
       </c>
       <c r="C153" s="22" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D153" s="22">
         <v>2018</v>
@@ -5552,7 +5554,7 @@
         <v>451</v>
       </c>
       <c r="C154" s="22" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D154" s="22">
         <v>2018</v>
@@ -5581,7 +5583,7 @@
         <v>452</v>
       </c>
       <c r="C155" s="22" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D155" s="22">
         <v>2018</v>
@@ -5610,7 +5612,7 @@
         <v>453</v>
       </c>
       <c r="C156" s="22" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D156" s="22">
         <v>2018</v>
@@ -5639,7 +5641,7 @@
         <v>454</v>
       </c>
       <c r="C157" s="22" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D157" s="22">
         <v>2018</v>
@@ -5668,7 +5670,7 @@
         <v>455</v>
       </c>
       <c r="C158" s="22" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D158" s="22">
         <v>2018</v>
@@ -5697,7 +5699,7 @@
         <v>456</v>
       </c>
       <c r="C159" s="22" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D159" s="22">
         <v>2018</v>
@@ -5726,7 +5728,7 @@
         <v>457</v>
       </c>
       <c r="C160" s="22" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D160" s="22">
         <v>2018</v>
@@ -5755,7 +5757,7 @@
         <v>458</v>
       </c>
       <c r="C161" s="22" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D161" s="22">
         <v>2018</v>
@@ -5784,7 +5786,7 @@
         <v>459</v>
       </c>
       <c r="C162" s="22" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D162" s="22">
         <v>2018</v>
@@ -5813,7 +5815,7 @@
         <v>460</v>
       </c>
       <c r="C163" s="22" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D163" s="22">
         <v>2018</v>
@@ -5842,7 +5844,7 @@
         <v>461</v>
       </c>
       <c r="C164" s="22" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D164" s="22">
         <v>2018</v>
@@ -5871,7 +5873,7 @@
         <v>462</v>
       </c>
       <c r="C165" s="22" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D165" s="22">
         <v>2018</v>
@@ -5900,7 +5902,7 @@
         <v>4</v>
       </c>
       <c r="C166" s="24" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D166" s="24">
         <v>2018</v>
@@ -5929,7 +5931,7 @@
         <v>0</v>
       </c>
       <c r="C167" s="24" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D167" s="24">
         <v>2018</v>
@@ -5958,7 +5960,7 @@
         <v>101</v>
       </c>
       <c r="C168" s="22" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D168" s="22">
         <v>2017</v>
@@ -5987,7 +5989,7 @@
         <v>102</v>
       </c>
       <c r="C169" s="22" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D169" s="22">
         <v>2017</v>
@@ -6016,7 +6018,7 @@
         <v>103</v>
       </c>
       <c r="C170" s="22" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D170" s="22">
         <v>2017</v>
@@ -6045,7 +6047,7 @@
         <v>151</v>
       </c>
       <c r="C171" s="22" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D171" s="22">
         <v>2017</v>
@@ -6074,7 +6076,7 @@
         <v>153</v>
       </c>
       <c r="C172" s="22" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="D172" s="22">
         <v>2017</v>
@@ -6103,7 +6105,7 @@
         <v>154</v>
       </c>
       <c r="C173" s="22" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D173" s="22">
         <v>2017</v>
@@ -6132,7 +6134,7 @@
         <v>155</v>
       </c>
       <c r="C174" s="22" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="D174" s="22">
         <v>2017</v>
@@ -6161,7 +6163,7 @@
         <v>157</v>
       </c>
       <c r="C175" s="22" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D175" s="22">
         <v>2017</v>
@@ -6190,7 +6192,7 @@
         <v>158</v>
       </c>
       <c r="C176" s="22" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D176" s="22">
         <v>2017</v>
@@ -6219,7 +6221,7 @@
         <v>159</v>
       </c>
       <c r="C177" s="22" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D177" s="22">
         <v>2017</v>
@@ -6248,7 +6250,7 @@
         <v>1</v>
       </c>
       <c r="C178" s="24" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D178" s="24">
         <v>2017</v>
@@ -6277,7 +6279,7 @@
         <v>241</v>
       </c>
       <c r="C179" s="22" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D179" s="22">
         <v>2017</v>
@@ -6306,7 +6308,7 @@
         <v>241001</v>
       </c>
       <c r="C180" s="22" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D180" s="22">
         <v>2017</v>
@@ -6373,7 +6375,7 @@
         <v>251</v>
       </c>
       <c r="C182" s="22" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="D182" s="22">
         <v>2017</v>
@@ -6402,7 +6404,7 @@
         <v>252</v>
       </c>
       <c r="C183" s="22" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="D183" s="22">
         <v>2017</v>
@@ -6431,7 +6433,7 @@
         <v>254</v>
       </c>
       <c r="C184" s="22" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D184" s="22">
         <v>2017</v>
@@ -6460,7 +6462,7 @@
         <v>255</v>
       </c>
       <c r="C185" s="22" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D185" s="22">
         <v>2017</v>
@@ -6489,7 +6491,7 @@
         <v>256</v>
       </c>
       <c r="C186" s="22" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="D186" s="22">
         <v>2017</v>
@@ -6518,7 +6520,7 @@
         <v>257</v>
       </c>
       <c r="C187" s="22" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D187" s="22">
         <v>2017</v>
@@ -6547,7 +6549,7 @@
         <v>2</v>
       </c>
       <c r="C188" s="24" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D188" s="24">
         <v>2017</v>
@@ -6576,7 +6578,7 @@
         <v>351</v>
       </c>
       <c r="C189" s="22" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="D189" s="22">
         <v>2017</v>
@@ -6605,7 +6607,7 @@
         <v>352</v>
       </c>
       <c r="C190" s="22" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="D190" s="22">
         <v>2017</v>
@@ -6634,7 +6636,7 @@
         <v>353</v>
       </c>
       <c r="C191" s="22" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="D191" s="22">
         <v>2017</v>
@@ -6663,7 +6665,7 @@
         <v>354</v>
       </c>
       <c r="C192" s="22" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="D192" s="22">
         <v>2017</v>
@@ -6692,7 +6694,7 @@
         <v>355</v>
       </c>
       <c r="C193" s="22" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="D193" s="22">
         <v>2017</v>
@@ -6721,7 +6723,7 @@
         <v>356</v>
       </c>
       <c r="C194" s="22" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="D194" s="22">
         <v>2017</v>
@@ -6750,7 +6752,7 @@
         <v>357</v>
       </c>
       <c r="C195" s="22" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D195" s="22">
         <v>2017</v>
@@ -6779,7 +6781,7 @@
         <v>358</v>
       </c>
       <c r="C196" s="22" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="D196" s="22">
         <v>2017</v>
@@ -6808,7 +6810,7 @@
         <v>359</v>
       </c>
       <c r="C197" s="22" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="D197" s="22">
         <v>2017</v>
@@ -6837,7 +6839,7 @@
         <v>360</v>
       </c>
       <c r="C198" s="22" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="D198" s="22">
         <v>2017</v>
@@ -6866,7 +6868,7 @@
         <v>361</v>
       </c>
       <c r="C199" s="22" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="D199" s="22">
         <v>2017</v>
@@ -6895,7 +6897,7 @@
         <v>3</v>
       </c>
       <c r="C200" s="24" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D200" s="24">
         <v>2017</v>
@@ -6924,7 +6926,7 @@
         <v>401</v>
       </c>
       <c r="C201" s="22" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="D201" s="22">
         <v>2017</v>
@@ -6953,7 +6955,7 @@
         <v>402</v>
       </c>
       <c r="C202" s="22" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="D202" s="22">
         <v>2017</v>
@@ -6982,7 +6984,7 @@
         <v>403</v>
       </c>
       <c r="C203" s="22" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="D203" s="22">
         <v>2017</v>
@@ -7011,7 +7013,7 @@
         <v>404</v>
       </c>
       <c r="C204" s="22" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="D204" s="22">
         <v>2017</v>
@@ -7040,7 +7042,7 @@
         <v>405</v>
       </c>
       <c r="C205" s="22" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="D205" s="22">
         <v>2017</v>
@@ -7069,7 +7071,7 @@
         <v>451</v>
       </c>
       <c r="C206" s="22" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="D206" s="22">
         <v>2017</v>
@@ -7098,7 +7100,7 @@
         <v>452</v>
       </c>
       <c r="C207" s="22" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="D207" s="22">
         <v>2017</v>
@@ -7127,7 +7129,7 @@
         <v>453</v>
       </c>
       <c r="C208" s="22" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="D208" s="22">
         <v>2017</v>
@@ -7156,7 +7158,7 @@
         <v>454</v>
       </c>
       <c r="C209" s="22" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="D209" s="22">
         <v>2017</v>
@@ -7185,7 +7187,7 @@
         <v>455</v>
       </c>
       <c r="C210" s="22" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="D210" s="22">
         <v>2017</v>
@@ -7214,7 +7216,7 @@
         <v>456</v>
       </c>
       <c r="C211" s="22" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="D211" s="22">
         <v>2017</v>
@@ -7243,7 +7245,7 @@
         <v>457</v>
       </c>
       <c r="C212" s="22" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="D212" s="22">
         <v>2017</v>
@@ -7272,7 +7274,7 @@
         <v>458</v>
       </c>
       <c r="C213" s="22" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="D213" s="22">
         <v>2017</v>
@@ -7301,7 +7303,7 @@
         <v>459</v>
       </c>
       <c r="C214" s="22" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="D214" s="22">
         <v>2017</v>
@@ -7330,7 +7332,7 @@
         <v>460</v>
       </c>
       <c r="C215" s="22" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="D215" s="22">
         <v>2017</v>
@@ -7359,7 +7361,7 @@
         <v>461</v>
       </c>
       <c r="C216" s="22" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="D216" s="22">
         <v>2017</v>
@@ -7388,7 +7390,7 @@
         <v>462</v>
       </c>
       <c r="C217" s="22" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="D217" s="22">
         <v>2017</v>
@@ -7417,7 +7419,7 @@
         <v>4</v>
       </c>
       <c r="C218" s="24" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D218" s="24">
         <v>2017</v>
@@ -7446,7 +7448,7 @@
         <v>0</v>
       </c>
       <c r="C219" s="24" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="D219" s="24">
         <v>2017</v>
@@ -7475,7 +7477,7 @@
         <v>101</v>
       </c>
       <c r="C220" s="22" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D220" s="22">
         <v>2016</v>
@@ -7504,7 +7506,7 @@
         <v>102</v>
       </c>
       <c r="C221" s="22" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D221" s="22">
         <v>2016</v>
@@ -7533,7 +7535,7 @@
         <v>103</v>
       </c>
       <c r="C222" s="22" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D222" s="22">
         <v>2016</v>
@@ -7562,7 +7564,7 @@
         <v>151</v>
       </c>
       <c r="C223" s="22" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D223" s="22">
         <v>2016</v>
@@ -7591,7 +7593,7 @@
         <v>153</v>
       </c>
       <c r="C224" s="22" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="D224" s="22">
         <v>2016</v>
@@ -7620,7 +7622,7 @@
         <v>154</v>
       </c>
       <c r="C225" s="22" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D225" s="22">
         <v>2016</v>
@@ -7649,7 +7651,7 @@
         <v>155</v>
       </c>
       <c r="C226" s="22" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="D226" s="22">
         <v>2016</v>
@@ -7678,7 +7680,7 @@
         <v>157</v>
       </c>
       <c r="C227" s="22" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D227" s="22">
         <v>2016</v>
@@ -7707,7 +7709,7 @@
         <v>158</v>
       </c>
       <c r="C228" s="22" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D228" s="22">
         <v>2016</v>
@@ -7736,7 +7738,7 @@
         <v>159</v>
       </c>
       <c r="C229" s="22" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D229" s="22">
         <v>2016</v>
@@ -7765,7 +7767,7 @@
         <v>1</v>
       </c>
       <c r="C230" s="24" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D230" s="24">
         <v>2016</v>
@@ -7794,7 +7796,7 @@
         <v>241</v>
       </c>
       <c r="C231" s="22" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D231" s="22">
         <v>2016</v>
@@ -7823,7 +7825,7 @@
         <v>241001</v>
       </c>
       <c r="C232" s="22" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D232" s="22">
         <v>2016</v>
@@ -7890,7 +7892,7 @@
         <v>251</v>
       </c>
       <c r="C234" s="22" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="D234" s="22">
         <v>2016</v>
@@ -7919,7 +7921,7 @@
         <v>252</v>
       </c>
       <c r="C235" s="22" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="D235" s="22">
         <v>2016</v>
@@ -7948,7 +7950,7 @@
         <v>254</v>
       </c>
       <c r="C236" s="22" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D236" s="22">
         <v>2016</v>
@@ -7977,7 +7979,7 @@
         <v>255</v>
       </c>
       <c r="C237" s="22" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D237" s="22">
         <v>2016</v>
@@ -8006,7 +8008,7 @@
         <v>256</v>
       </c>
       <c r="C238" s="22" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="D238" s="22">
         <v>2016</v>
@@ -8035,7 +8037,7 @@
         <v>257</v>
       </c>
       <c r="C239" s="22" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D239" s="22">
         <v>2016</v>
@@ -8064,7 +8066,7 @@
         <v>2</v>
       </c>
       <c r="C240" s="24" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D240" s="24">
         <v>2016</v>
@@ -8093,7 +8095,7 @@
         <v>351</v>
       </c>
       <c r="C241" s="22" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="D241" s="22">
         <v>2016</v>
@@ -8122,7 +8124,7 @@
         <v>352</v>
       </c>
       <c r="C242" s="22" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="D242" s="22">
         <v>2016</v>
@@ -8151,7 +8153,7 @@
         <v>353</v>
       </c>
       <c r="C243" s="22" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="D243" s="22">
         <v>2016</v>
@@ -8180,7 +8182,7 @@
         <v>354</v>
       </c>
       <c r="C244" s="22" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="D244" s="22">
         <v>2016</v>
@@ -8209,7 +8211,7 @@
         <v>355</v>
       </c>
       <c r="C245" s="22" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="D245" s="22">
         <v>2016</v>
@@ -8238,7 +8240,7 @@
         <v>356</v>
       </c>
       <c r="C246" s="22" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="D246" s="22">
         <v>2016</v>
@@ -8267,7 +8269,7 @@
         <v>357</v>
       </c>
       <c r="C247" s="22" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D247" s="22">
         <v>2016</v>
@@ -8296,7 +8298,7 @@
         <v>358</v>
       </c>
       <c r="C248" s="22" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="D248" s="22">
         <v>2016</v>
@@ -8325,7 +8327,7 @@
         <v>359</v>
       </c>
       <c r="C249" s="22" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="D249" s="22">
         <v>2016</v>
@@ -8354,7 +8356,7 @@
         <v>360</v>
       </c>
       <c r="C250" s="22" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="D250" s="22">
         <v>2016</v>
@@ -8383,7 +8385,7 @@
         <v>361</v>
       </c>
       <c r="C251" s="22" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="D251" s="22">
         <v>2016</v>
@@ -8412,7 +8414,7 @@
         <v>3</v>
       </c>
       <c r="C252" s="24" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D252" s="24">
         <v>2016</v>
@@ -8441,7 +8443,7 @@
         <v>401</v>
       </c>
       <c r="C253" s="22" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="D253" s="22">
         <v>2016</v>
@@ -8470,7 +8472,7 @@
         <v>402</v>
       </c>
       <c r="C254" s="22" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="D254" s="22">
         <v>2016</v>
@@ -8499,7 +8501,7 @@
         <v>403</v>
       </c>
       <c r="C255" s="22" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="D255" s="22">
         <v>2016</v>
@@ -8528,7 +8530,7 @@
         <v>404</v>
       </c>
       <c r="C256" s="22" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="D256" s="22">
         <v>2016</v>
@@ -8557,7 +8559,7 @@
         <v>405</v>
       </c>
       <c r="C257" s="22" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="D257" s="22">
         <v>2016</v>
@@ -8586,7 +8588,7 @@
         <v>451</v>
       </c>
       <c r="C258" s="22" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="D258" s="22">
         <v>2016</v>
@@ -8615,7 +8617,7 @@
         <v>452</v>
       </c>
       <c r="C259" s="22" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="D259" s="22">
         <v>2016</v>
@@ -8644,7 +8646,7 @@
         <v>453</v>
       </c>
       <c r="C260" s="22" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="D260" s="22">
         <v>2016</v>
@@ -8673,7 +8675,7 @@
         <v>454</v>
       </c>
       <c r="C261" s="22" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="D261" s="22">
         <v>2016</v>
@@ -8702,7 +8704,7 @@
         <v>455</v>
       </c>
       <c r="C262" s="22" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="D262" s="22">
         <v>2016</v>
@@ -8731,7 +8733,7 @@
         <v>456</v>
       </c>
       <c r="C263" s="22" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="D263" s="22">
         <v>2016</v>
@@ -8760,7 +8762,7 @@
         <v>457</v>
       </c>
       <c r="C264" s="22" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="D264" s="22">
         <v>2016</v>
@@ -8789,7 +8791,7 @@
         <v>458</v>
       </c>
       <c r="C265" s="22" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="D265" s="22">
         <v>2016</v>
@@ -8818,7 +8820,7 @@
         <v>459</v>
       </c>
       <c r="C266" s="22" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="D266" s="22">
         <v>2016</v>
@@ -8847,7 +8849,7 @@
         <v>460</v>
       </c>
       <c r="C267" s="22" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="D267" s="22">
         <v>2016</v>
@@ -8876,7 +8878,7 @@
         <v>461</v>
       </c>
       <c r="C268" s="22" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="D268" s="22">
         <v>2016</v>
@@ -8905,7 +8907,7 @@
         <v>462</v>
       </c>
       <c r="C269" s="22" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="D269" s="22">
         <v>2016</v>
@@ -8934,7 +8936,7 @@
         <v>4</v>
       </c>
       <c r="C270" s="24" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D270" s="24">
         <v>2016</v>
@@ -8963,7 +8965,7 @@
         <v>0</v>
       </c>
       <c r="C271" s="24" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="D271" s="24">
         <v>2016</v>
@@ -8992,7 +8994,7 @@
         <v>101</v>
       </c>
       <c r="C272" s="26" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D272" s="22">
         <v>2015</v>
@@ -9021,7 +9023,7 @@
         <v>102</v>
       </c>
       <c r="C273" s="26" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D273" s="22">
         <v>2015</v>
@@ -9050,7 +9052,7 @@
         <v>103</v>
       </c>
       <c r="C274" s="26" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D274" s="22">
         <v>2015</v>
@@ -9079,7 +9081,7 @@
         <v>151</v>
       </c>
       <c r="C275" s="26" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D275" s="22">
         <v>2015</v>
@@ -9108,7 +9110,7 @@
         <v>153</v>
       </c>
       <c r="C276" s="26" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="D276" s="22">
         <v>2015</v>
@@ -9137,7 +9139,7 @@
         <v>154</v>
       </c>
       <c r="C277" s="26" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D277" s="22">
         <v>2015</v>
@@ -9166,7 +9168,7 @@
         <v>155</v>
       </c>
       <c r="C278" s="26" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="D278" s="22">
         <v>2015</v>
@@ -9195,7 +9197,7 @@
         <v>157</v>
       </c>
       <c r="C279" s="26" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D279" s="22">
         <v>2015</v>
@@ -9224,7 +9226,7 @@
         <v>158</v>
       </c>
       <c r="C280" s="26" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D280" s="22">
         <v>2015</v>
@@ -9291,7 +9293,7 @@
         <v>1</v>
       </c>
       <c r="C282" s="24" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D282" s="24">
         <v>2015</v>
@@ -9320,7 +9322,7 @@
         <v>241</v>
       </c>
       <c r="C283" s="26" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D283" s="22">
         <v>2015</v>
@@ -9349,7 +9351,7 @@
         <v>241001</v>
       </c>
       <c r="C284" s="22" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D284" s="22">
         <v>2015</v>
@@ -9416,7 +9418,7 @@
         <v>251</v>
       </c>
       <c r="C286" s="26" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="D286" s="22">
         <v>2015</v>
@@ -9445,7 +9447,7 @@
         <v>252</v>
       </c>
       <c r="C287" s="26" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="D287" s="22">
         <v>2015</v>
@@ -9474,7 +9476,7 @@
         <v>254</v>
       </c>
       <c r="C288" s="26" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D288" s="22">
         <v>2015</v>
@@ -9503,7 +9505,7 @@
         <v>255</v>
       </c>
       <c r="C289" s="26" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D289" s="22">
         <v>2015</v>
@@ -9532,7 +9534,7 @@
         <v>256</v>
       </c>
       <c r="C290" s="26" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="D290" s="22">
         <v>2015</v>
@@ -9561,7 +9563,7 @@
         <v>257</v>
       </c>
       <c r="C291" s="26" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D291" s="22">
         <v>2015</v>
@@ -9590,7 +9592,7 @@
         <v>2</v>
       </c>
       <c r="C292" s="24" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D292" s="24">
         <v>2015</v>
@@ -9619,7 +9621,7 @@
         <v>351</v>
       </c>
       <c r="C293" s="26" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="D293" s="22">
         <v>2015</v>
@@ -9648,7 +9650,7 @@
         <v>352</v>
       </c>
       <c r="C294" s="26" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="D294" s="22">
         <v>2015</v>
@@ -9677,7 +9679,7 @@
         <v>353</v>
       </c>
       <c r="C295" s="26" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="D295" s="22">
         <v>2015</v>
@@ -9706,7 +9708,7 @@
         <v>354</v>
       </c>
       <c r="C296" s="26" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="D296" s="22">
         <v>2015</v>
@@ -9735,7 +9737,7 @@
         <v>355</v>
       </c>
       <c r="C297" s="26" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="D297" s="22">
         <v>2015</v>
@@ -9764,7 +9766,7 @@
         <v>356</v>
       </c>
       <c r="C298" s="26" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="D298" s="22">
         <v>2015</v>
@@ -9793,7 +9795,7 @@
         <v>357</v>
       </c>
       <c r="C299" s="26" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D299" s="22">
         <v>2015</v>
@@ -9822,7 +9824,7 @@
         <v>358</v>
       </c>
       <c r="C300" s="26" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="D300" s="22">
         <v>2015</v>
@@ -9851,7 +9853,7 @@
         <v>359</v>
       </c>
       <c r="C301" s="26" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="D301" s="22">
         <v>2015</v>
@@ -9880,7 +9882,7 @@
         <v>360</v>
       </c>
       <c r="C302" s="26" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="D302" s="22">
         <v>2015</v>
@@ -9909,7 +9911,7 @@
         <v>361</v>
       </c>
       <c r="C303" s="26" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="D303" s="22">
         <v>2015</v>
@@ -9938,7 +9940,7 @@
         <v>3</v>
       </c>
       <c r="C304" s="24" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D304" s="24">
         <v>2015</v>
@@ -9967,7 +9969,7 @@
         <v>401</v>
       </c>
       <c r="C305" s="26" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="D305" s="22">
         <v>2015</v>
@@ -9996,7 +9998,7 @@
         <v>402</v>
       </c>
       <c r="C306" s="26" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="D306" s="22">
         <v>2015</v>
@@ -10025,7 +10027,7 @@
         <v>403</v>
       </c>
       <c r="C307" s="26" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="D307" s="22">
         <v>2015</v>
@@ -10054,7 +10056,7 @@
         <v>404</v>
       </c>
       <c r="C308" s="26" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="D308" s="22">
         <v>2015</v>
@@ -10083,7 +10085,7 @@
         <v>405</v>
       </c>
       <c r="C309" s="26" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="D309" s="22">
         <v>2015</v>
@@ -10112,7 +10114,7 @@
         <v>451</v>
       </c>
       <c r="C310" s="26" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="D310" s="22">
         <v>2015</v>
@@ -10141,7 +10143,7 @@
         <v>452</v>
       </c>
       <c r="C311" s="26" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="D311" s="22">
         <v>2015</v>
@@ -10170,7 +10172,7 @@
         <v>453</v>
       </c>
       <c r="C312" s="26" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="D312" s="22">
         <v>2015</v>
@@ -10199,7 +10201,7 @@
         <v>454</v>
       </c>
       <c r="C313" s="26" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="D313" s="22">
         <v>2015</v>
@@ -10228,7 +10230,7 @@
         <v>455</v>
       </c>
       <c r="C314" s="26" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="D314" s="22">
         <v>2015</v>
@@ -10257,7 +10259,7 @@
         <v>456</v>
       </c>
       <c r="C315" s="26" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="D315" s="22">
         <v>2015</v>
@@ -10286,7 +10288,7 @@
         <v>457</v>
       </c>
       <c r="C316" s="26" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="D316" s="22">
         <v>2015</v>
@@ -10315,7 +10317,7 @@
         <v>458</v>
       </c>
       <c r="C317" s="26" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="D317" s="22">
         <v>2015</v>
@@ -10344,7 +10346,7 @@
         <v>459</v>
       </c>
       <c r="C318" s="26" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="D318" s="22">
         <v>2015</v>
@@ -10373,7 +10375,7 @@
         <v>460</v>
       </c>
       <c r="C319" s="26" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="D319" s="22">
         <v>2015</v>
@@ -10402,7 +10404,7 @@
         <v>461</v>
       </c>
       <c r="C320" s="26" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="D320" s="22">
         <v>2015</v>
@@ -10431,7 +10433,7 @@
         <v>462</v>
       </c>
       <c r="C321" s="26" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="D321" s="22">
         <v>2015</v>
@@ -10460,7 +10462,7 @@
         <v>4</v>
       </c>
       <c r="C322" s="24" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D322" s="24">
         <v>2015</v>
@@ -10489,7 +10491,7 @@
         <v>0</v>
       </c>
       <c r="C323" s="28" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="D323" s="24">
         <v>2015</v>
@@ -10518,7 +10520,7 @@
         <v>101</v>
       </c>
       <c r="C324" s="26" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D324" s="22">
         <v>2014</v>
@@ -10547,7 +10549,7 @@
         <v>102</v>
       </c>
       <c r="C325" s="26" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D325" s="22">
         <v>2014</v>
@@ -10576,7 +10578,7 @@
         <v>103</v>
       </c>
       <c r="C326" s="26" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D326" s="22">
         <v>2014</v>
@@ -10605,7 +10607,7 @@
         <v>151</v>
       </c>
       <c r="C327" s="26" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D327" s="22">
         <v>2014</v>
@@ -10634,7 +10636,7 @@
         <v>153</v>
       </c>
       <c r="C328" s="26" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="D328" s="22">
         <v>2014</v>
@@ -10663,7 +10665,7 @@
         <v>154</v>
       </c>
       <c r="C329" s="26" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D329" s="22">
         <v>2014</v>
@@ -10692,7 +10694,7 @@
         <v>155</v>
       </c>
       <c r="C330" s="26" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="D330" s="22">
         <v>2014</v>
@@ -10721,7 +10723,7 @@
         <v>157</v>
       </c>
       <c r="C331" s="26" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D331" s="22">
         <v>2014</v>
@@ -10750,7 +10752,7 @@
         <v>158</v>
       </c>
       <c r="C332" s="26" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D332" s="22">
         <v>2014</v>
@@ -10817,7 +10819,7 @@
         <v>1</v>
       </c>
       <c r="C334" s="24" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D334" s="24">
         <v>2014</v>
@@ -10846,7 +10848,7 @@
         <v>241</v>
       </c>
       <c r="C335" s="26" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D335" s="22">
         <v>2014</v>
@@ -10875,7 +10877,7 @@
         <v>241001</v>
       </c>
       <c r="C336" s="22" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D336" s="22">
         <v>2014</v>
@@ -10942,7 +10944,7 @@
         <v>251</v>
       </c>
       <c r="C338" s="26" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="D338" s="22">
         <v>2014</v>
@@ -10971,7 +10973,7 @@
         <v>252</v>
       </c>
       <c r="C339" s="26" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="D339" s="22">
         <v>2014</v>
@@ -11000,7 +11002,7 @@
         <v>254</v>
       </c>
       <c r="C340" s="26" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D340" s="22">
         <v>2014</v>
@@ -11029,7 +11031,7 @@
         <v>255</v>
       </c>
       <c r="C341" s="26" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D341" s="22">
         <v>2014</v>
@@ -11058,7 +11060,7 @@
         <v>256</v>
       </c>
       <c r="C342" s="26" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="D342" s="22">
         <v>2014</v>
@@ -11087,7 +11089,7 @@
         <v>257</v>
       </c>
       <c r="C343" s="26" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D343" s="22">
         <v>2014</v>
@@ -11116,7 +11118,7 @@
         <v>2</v>
       </c>
       <c r="C344" s="24" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D344" s="24">
         <v>2014</v>
@@ -11145,7 +11147,7 @@
         <v>351</v>
       </c>
       <c r="C345" s="26" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="D345" s="22">
         <v>2014</v>
@@ -11174,7 +11176,7 @@
         <v>352</v>
       </c>
       <c r="C346" s="26" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="D346" s="22">
         <v>2014</v>
@@ -11203,7 +11205,7 @@
         <v>353</v>
       </c>
       <c r="C347" s="26" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="D347" s="22">
         <v>2014</v>
@@ -11232,7 +11234,7 @@
         <v>354</v>
       </c>
       <c r="C348" s="26" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="D348" s="22">
         <v>2014</v>
@@ -11261,7 +11263,7 @@
         <v>355</v>
       </c>
       <c r="C349" s="26" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="D349" s="22">
         <v>2014</v>
@@ -11290,7 +11292,7 @@
         <v>356</v>
       </c>
       <c r="C350" s="26" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="D350" s="22">
         <v>2014</v>
@@ -11319,7 +11321,7 @@
         <v>357</v>
       </c>
       <c r="C351" s="26" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D351" s="22">
         <v>2014</v>
@@ -11348,7 +11350,7 @@
         <v>358</v>
       </c>
       <c r="C352" s="26" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="D352" s="22">
         <v>2014</v>
@@ -11377,7 +11379,7 @@
         <v>359</v>
       </c>
       <c r="C353" s="26" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="D353" s="22">
         <v>2014</v>
@@ -11406,7 +11408,7 @@
         <v>360</v>
       </c>
       <c r="C354" s="26" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="D354" s="22">
         <v>2014</v>
@@ -11435,7 +11437,7 @@
         <v>361</v>
       </c>
       <c r="C355" s="26" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="D355" s="22">
         <v>2014</v>
@@ -11464,7 +11466,7 @@
         <v>3</v>
       </c>
       <c r="C356" s="24" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D356" s="24">
         <v>2014</v>
@@ -11493,7 +11495,7 @@
         <v>401</v>
       </c>
       <c r="C357" s="26" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="D357" s="22">
         <v>2014</v>
@@ -11522,7 +11524,7 @@
         <v>402</v>
       </c>
       <c r="C358" s="26" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="D358" s="22">
         <v>2014</v>
@@ -11551,7 +11553,7 @@
         <v>403</v>
       </c>
       <c r="C359" s="26" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="D359" s="22">
         <v>2014</v>
@@ -11580,7 +11582,7 @@
         <v>404</v>
       </c>
       <c r="C360" s="26" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="D360" s="22">
         <v>2014</v>
@@ -11609,7 +11611,7 @@
         <v>405</v>
       </c>
       <c r="C361" s="26" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="D361" s="22">
         <v>2014</v>
@@ -11638,7 +11640,7 @@
         <v>451</v>
       </c>
       <c r="C362" s="26" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="D362" s="22">
         <v>2014</v>
@@ -11667,7 +11669,7 @@
         <v>452</v>
       </c>
       <c r="C363" s="26" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="D363" s="22">
         <v>2014</v>
@@ -11696,7 +11698,7 @@
         <v>453</v>
       </c>
       <c r="C364" s="26" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="D364" s="22">
         <v>2014</v>
@@ -11725,7 +11727,7 @@
         <v>454</v>
       </c>
       <c r="C365" s="26" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="D365" s="22">
         <v>2014</v>
@@ -11754,7 +11756,7 @@
         <v>455</v>
       </c>
       <c r="C366" s="26" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="D366" s="22">
         <v>2014</v>
@@ -11783,7 +11785,7 @@
         <v>456</v>
       </c>
       <c r="C367" s="26" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="D367" s="22">
         <v>2014</v>
@@ -11812,7 +11814,7 @@
         <v>457</v>
       </c>
       <c r="C368" s="26" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="D368" s="22">
         <v>2014</v>
@@ -11841,7 +11843,7 @@
         <v>458</v>
       </c>
       <c r="C369" s="26" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="D369" s="22">
         <v>2014</v>
@@ -11870,7 +11872,7 @@
         <v>459</v>
       </c>
       <c r="C370" s="26" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="D370" s="22">
         <v>2014</v>
@@ -11899,7 +11901,7 @@
         <v>460</v>
       </c>
       <c r="C371" s="26" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="D371" s="22">
         <v>2014</v>
@@ -11928,7 +11930,7 @@
         <v>461</v>
       </c>
       <c r="C372" s="26" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="D372" s="22">
         <v>2014</v>
@@ -11957,7 +11959,7 @@
         <v>462</v>
       </c>
       <c r="C373" s="26" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="D373" s="22">
         <v>2014</v>
@@ -11986,7 +11988,7 @@
         <v>4</v>
       </c>
       <c r="C374" s="24" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D374" s="24">
         <v>2014</v>
@@ -12015,7 +12017,7 @@
         <v>0</v>
       </c>
       <c r="C375" s="28" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="D375" s="24">
         <v>2014</v>
@@ -12044,7 +12046,7 @@
     </row>
     <row r="377" spans="2:10" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C377" s="34" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="D377" s="34"/>
       <c r="E377" s="34"/>
@@ -12066,7 +12068,7 @@
     </row>
     <row r="379" spans="2:10" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C379" s="31" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="D379" s="32"/>
       <c r="E379" s="32"/>
@@ -12088,7 +12090,7 @@
     </row>
     <row r="381" spans="2:10" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C381" s="31" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="D381" s="31"/>
       <c r="E381" s="31"/>
@@ -12100,7 +12102,7 @@
     </row>
     <row r="382" spans="2:10" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C382" s="31" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="D382" s="31"/>
       <c r="E382" s="31"/>
@@ -12112,7 +12114,7 @@
     </row>
     <row r="383" spans="2:10" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C383" s="31" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="D383" s="31"/>
       <c r="E383" s="31"/>
@@ -12124,7 +12126,7 @@
     </row>
     <row r="384" spans="2:10" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C384" s="33" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="D384" s="31"/>
       <c r="E384" s="31"/>

</xml_diff>

<commit_message>
Deploying to gh-pages from  @ 2a0e43cae02364e85946d47a1eb6eae7392fdee0 🚀
</commit_message>
<xml_diff>
--- a/assets/excel/2022_6-2-2.xlsx
+++ b/assets/excel/2022_6-2-2.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="S:\Hannover\Dez15-Uebergreifende-Analysen\Projekte\Integrationsmonitoring\github\MT_Site\assets\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F2C8686-BB0E-4D2A-8695-BBA6D212F225}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{83ED14CE-B914-45AD-AF28-1FD958F01048}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="14010" xr2:uid="{6D20BA34-5F99-4BCC-BC15-D54A156181FF}"/>
   </bookViews>
@@ -396,7 +396,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="11" x14ac:knownFonts="1">
+  <fonts count="12" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -456,6 +456,11 @@
       <sz val="6"/>
       <color theme="10"/>
       <name val="NDSFrutiger 45 Light"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="NDSFrutiger 55 Roman"/>
     </font>
   </fonts>
   <fills count="3">
@@ -615,7 +620,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="49">
+  <cellXfs count="50">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
@@ -739,6 +744,9 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -1279,9 +1287,7 @@
   <sheetPr codeName="Tabelle1"/>
   <dimension ref="B1:O384"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
-    </sheetView>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="205" zoomScaleNormal="205" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1721,7 +1727,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="22" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:10" s="49" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B22" s="23">
         <v>1</v>
       </c>
@@ -1731,22 +1737,22 @@
       <c r="D22" s="24">
         <v>2020</v>
       </c>
-      <c r="E22" s="22">
+      <c r="E22" s="24">
         <v>90</v>
       </c>
-      <c r="F22" s="22">
+      <c r="F22" s="24">
         <v>71</v>
       </c>
-      <c r="G22" s="22">
+      <c r="G22" s="24">
         <v>26</v>
       </c>
-      <c r="H22" s="22">
+      <c r="H22" s="24">
         <v>527</v>
       </c>
-      <c r="I22" s="22">
+      <c r="I22" s="24">
         <v>259</v>
       </c>
-      <c r="J22" s="22">
+      <c r="J22" s="24">
         <v>187</v>
       </c>
     </row>
@@ -2011,7 +2017,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="32" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="32" spans="2:10" s="49" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B32" s="23">
         <v>2</v>
       </c>
@@ -2021,22 +2027,22 @@
       <c r="D32" s="24">
         <v>2020</v>
       </c>
-      <c r="E32" s="22">
+      <c r="E32" s="24">
         <v>110</v>
       </c>
-      <c r="F32" s="22">
+      <c r="F32" s="24">
         <v>76</v>
       </c>
-      <c r="G32" s="22">
+      <c r="G32" s="24">
         <v>31</v>
       </c>
-      <c r="H32" s="22">
+      <c r="H32" s="24">
         <v>608</v>
       </c>
-      <c r="I32" s="22">
+      <c r="I32" s="24">
         <v>321</v>
       </c>
-      <c r="J32" s="22">
+      <c r="J32" s="24">
         <v>292</v>
       </c>
     </row>
@@ -2359,7 +2365,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="44" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="44" spans="2:10" s="49" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B44" s="23">
         <v>3</v>
       </c>
@@ -2369,22 +2375,22 @@
       <c r="D44" s="24">
         <v>2020</v>
       </c>
-      <c r="E44" s="22">
+      <c r="E44" s="24">
         <v>75</v>
       </c>
-      <c r="F44" s="22">
+      <c r="F44" s="24">
         <v>59</v>
       </c>
-      <c r="G44" s="22">
+      <c r="G44" s="24">
         <v>24</v>
       </c>
-      <c r="H44" s="22">
+      <c r="H44" s="24">
         <v>494</v>
       </c>
-      <c r="I44" s="22">
+      <c r="I44" s="24">
         <v>258</v>
       </c>
-      <c r="J44" s="22">
+      <c r="J44" s="24">
         <v>200</v>
       </c>
     </row>
@@ -2881,7 +2887,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="62" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="62" spans="2:10" s="49" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B62" s="23">
         <v>4</v>
       </c>
@@ -2891,26 +2897,26 @@
       <c r="D62" s="24">
         <v>2020</v>
       </c>
-      <c r="E62" s="22">
+      <c r="E62" s="24">
         <v>74</v>
       </c>
-      <c r="F62" s="22">
+      <c r="F62" s="24">
         <v>62</v>
       </c>
-      <c r="G62" s="22">
+      <c r="G62" s="24">
         <v>27</v>
       </c>
-      <c r="H62" s="22">
+      <c r="H62" s="24">
         <v>407</v>
       </c>
-      <c r="I62" s="22">
+      <c r="I62" s="24">
         <v>211</v>
       </c>
-      <c r="J62" s="22">
+      <c r="J62" s="24">
         <v>200</v>
       </c>
     </row>
-    <row r="63" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="63" spans="2:10" s="49" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B63" s="23">
         <v>0</v>
       </c>
@@ -2920,22 +2926,22 @@
       <c r="D63" s="24">
         <v>2020</v>
       </c>
-      <c r="E63" s="22">
+      <c r="E63" s="24">
         <v>87</v>
       </c>
-      <c r="F63" s="22">
+      <c r="F63" s="24">
         <v>67</v>
       </c>
-      <c r="G63" s="22">
+      <c r="G63" s="24">
         <v>27</v>
       </c>
-      <c r="H63" s="22">
+      <c r="H63" s="24">
         <v>504</v>
       </c>
-      <c r="I63" s="22">
+      <c r="I63" s="24">
         <v>263</v>
       </c>
-      <c r="J63" s="22">
+      <c r="J63" s="24">
         <v>233</v>
       </c>
     </row>
@@ -12150,5 +12156,6 @@
     <hyperlink ref="C384" r:id="rId1" xr:uid="{B77B2D50-DED9-4324-9352-4F7A2E82FE72}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>